<commit_message>
FEAT; added data (1)
</commit_message>
<xml_diff>
--- a/data/shop_data.xlsx
+++ b/data/shop_data.xlsx
@@ -942,16 +942,10 @@
     <t>https://kko.kakao.com/bZnhE89-q2</t>
   </si>
   <si>
-    <t>프랭크커ㅠㅣㄴ바 첨단점</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
-      </rPr>
-      <t>https://naver.me/GplQq2TN</t>
-    </r>
+    <t>프랭크커핀바 첨단점</t>
+  </si>
+  <si>
+    <t>https://naver.me/GplQq2TN</t>
   </si>
   <si>
     <t>https://kko.kakao.com/P9usYXrm8r</t>
@@ -4695,7 +4689,7 @@
       <c r="R47" s="5">
         <v>4.0</v>
       </c>
-      <c r="S47" s="9" t="s">
+      <c r="S47" s="12" t="s">
         <v>224</v>
       </c>
       <c r="T47" s="9" t="s">

</xml_diff>